<commit_message>
Change the instruction xlsx file
</commit_message>
<xml_diff>
--- a/project/main/xlsx_files/instruction.xlsx
+++ b/project/main/xlsx_files/instruction.xlsx
@@ -139,7 +139,7 @@
     <t>№</t>
   </si>
   <si>
-    <t>От</t>
+    <t>На</t>
   </si>
   <si>
     <t>с ЕГН</t>
@@ -1806,49 +1806,49 @@
     <row r="997" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
     <mergeCell ref="F24:I24"/>
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A27:I27"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="G44:I44"/>
     <mergeCell ref="B32:E32"/>
-    <mergeCell ref="G32:I32"/>
     <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B34:I34"/>
     <mergeCell ref="A36:I36"/>
     <mergeCell ref="A38:I38"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="D40:F40"/>
     <mergeCell ref="G40:H40"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="G43:H43"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>